<commit_message>
Output of version 0.18.1
</commit_message>
<xml_diff>
--- a/Output/Excel/features.xlsx
+++ b/Output/Excel/features.xlsx
@@ -16,18 +16,19 @@
     <x:sheet name="STEPARGUMENTTRANSFORMATIONS" sheetId="9" r:id="rId9"/>
     <x:sheet name="CALLINGSTEPSFROMSTEPDEFINITIONS" sheetId="10" r:id="rId10"/>
     <x:sheet name="ATTRIBUTEOVERLOADING" sheetId="11" r:id="rId11"/>
-    <x:sheet name="SHOWTHECOMPARETOFEATURE" sheetId="12" r:id="rId12"/>
-    <x:sheet name="SHOWINGTABLEUSAGE" sheetId="13" r:id="rId13"/>
-    <x:sheet name="SHOWTHEUSEOFBACKGROUND" sheetId="14" r:id="rId14"/>
-    <x:sheet name="SCENARIOOUTLINE" sheetId="15" r:id="rId15"/>
-    <x:sheet name="FEATURECONTEXTFEATURES" sheetId="16" r:id="rId16"/>
-    <x:sheet name="SCENARIOCONTEXTFEATURES" sheetId="17" r:id="rId17"/>
-    <x:sheet name="TAGDEMONSTRATOR" sheetId="18" r:id="rId18"/>
-    <x:sheet name="ADDITION" sheetId="19" r:id="rId19"/>
-    <x:sheet name="THETESTRUNNERISNOT(VERY)IMPORTA" sheetId="20" r:id="rId20"/>
-    <x:sheet name="SHOWINGBASICGHERKINSYNTAX" sheetId="21" r:id="rId21"/>
-    <x:sheet name="TRIGONOMETRY" sheetId="22" r:id="rId22"/>
-    <x:sheet name="ARITHMETIC" sheetId="23" r:id="rId23"/>
+    <x:sheet name="SUMMERING" sheetId="12" r:id="rId12"/>
+    <x:sheet name="SHOWTHECOMPARETOFEATURE" sheetId="13" r:id="rId13"/>
+    <x:sheet name="SHOWINGTABLEUSAGE" sheetId="14" r:id="rId14"/>
+    <x:sheet name="SHOWTHEUSEOFBACKGROUND" sheetId="15" r:id="rId15"/>
+    <x:sheet name="SCENARIOOUTLINE" sheetId="16" r:id="rId16"/>
+    <x:sheet name="FEATURECONTEXTFEATURES" sheetId="17" r:id="rId17"/>
+    <x:sheet name="SCENARIOCONTEXTFEATURES" sheetId="18" r:id="rId18"/>
+    <x:sheet name="TAGDEMONSTRATOR" sheetId="19" r:id="rId19"/>
+    <x:sheet name="ADDITION" sheetId="20" r:id="rId20"/>
+    <x:sheet name="THETESTRUNNERISNOT(VERY)IMPORTA" sheetId="21" r:id="rId21"/>
+    <x:sheet name="SHOWINGBASICGHERKINSYNTAX" sheetId="22" r:id="rId22"/>
+    <x:sheet name="TRIGONOMETRY" sheetId="23" r:id="rId23"/>
+    <x:sheet name="ARITHMETIC" sheetId="24" r:id="rId24"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
   <x:si>
     <x:t>Clearing Screen</x:t>
   </x:si>
@@ -434,6 +435,41 @@
     <x:t>the number 3 is odd</x:t>
   </x:si>
   <x:si>
+    <x:t>Summering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>För att slippa att göra dumma fel
+Som räknare
+Vill jag kunna lägga summera</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Summera 5 och 7 ska vara 12</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Givet </x:t>
+  </x:si>
+  <x:si>
+    <x:t>att jag har knappat in 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Och </x:t>
+  </x:si>
+  <x:si>
+    <x:t>att jag har knappat in 7</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">När </x:t>
+  </x:si>
+  <x:si>
+    <x:t>jag summerar</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Så </x:t>
+  </x:si>
+  <x:si>
+    <x:t>ska resultatet vara 12</x:t>
+  </x:si>
+  <x:si>
     <x:t>Show the compare to feature</x:t>
   </x:si>
   <x:si>
@@ -979,6 +1015,9 @@
   </x:si>
   <x:si>
     <x:t>06 Compare To Assist</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07 Svenska</x:t>
   </x:si>
   <x:si>
     <x:t>08 Attribute Overloading</x:t>
@@ -1459,7 +1498,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E42"/>
+  <x:dimension ref="A1:E44"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1467,211 +1506,221 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="1" t="s">
-        <x:v>279</x:v>
+        <x:v>290</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="B2" s="7" t="s">
-        <x:v>266</x:v>
+        <x:v>277</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="B3" s="7" t="s">
-        <x:v>254</x:v>
+        <x:v>265</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="B4" s="1" t="s">
-        <x:v>280</x:v>
+        <x:v>291</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="C5" s="7" t="s">
-        <x:v>244</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="B6" s="1" t="s">
-        <x:v>281</x:v>
+        <x:v>292</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="C7" s="7" t="s">
-        <x:v>238</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="B8" s="1" t="s">
-        <x:v>282</x:v>
+        <x:v>293</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="C9" s="7" t="s">
-        <x:v>225</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="C10" s="7" t="s">
-        <x:v>206</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="B11" s="1" t="s">
-        <x:v>283</x:v>
+        <x:v>294</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="C12" s="7" t="s">
-        <x:v>188</x:v>
+        <x:v>199</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="B13" s="1" t="s">
-        <x:v>284</x:v>
+        <x:v>295</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="C14" s="7" t="s">
-        <x:v>171</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="B15" s="1" t="s">
-        <x:v>285</x:v>
+        <x:v>296</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="C16" s="7" t="s">
-        <x:v>160</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="B17" s="1" t="s">
-        <x:v>286</x:v>
+        <x:v>297</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="C18" s="7" t="s">
-        <x:v>152</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
       <x:c r="B19" s="1" t="s">
-        <x:v>287</x:v>
+        <x:v>298</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="C20" s="7" t="s">
-        <x:v>138</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
       <x:c r="B21" s="1" t="s">
-        <x:v>288</x:v>
+        <x:v>299</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
       <x:c r="C22" s="7" t="s">
-        <x:v>115</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
       <x:c r="B23" s="1" t="s">
-        <x:v>289</x:v>
+        <x:v>300</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
       <x:c r="C24" s="7" t="s">
-        <x:v>104</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
       <x:c r="B25" s="1" t="s">
-        <x:v>290</x:v>
+        <x:v>301</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
       <x:c r="C26" s="7" t="s">
-        <x:v>93</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
       <x:c r="B27" s="1" t="s">
-        <x:v>291</x:v>
+        <x:v>302</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5">
       <x:c r="C28" s="7" t="s">
-        <x:v>87</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
       <x:c r="B29" s="1" t="s">
-        <x:v>292</x:v>
+        <x:v>303</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:5">
       <x:c r="C30" s="7" t="s">
-        <x:v>71</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
       <x:c r="B31" s="1" t="s">
-        <x:v>293</x:v>
+        <x:v>304</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:5">
-      <x:c r="C32" s="1" t="s">
-        <x:v>294</x:v>
+      <x:c r="C32" s="7" t="s">
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:5">
-      <x:c r="D33" s="1" t="s">
-        <x:v>295</x:v>
+      <x:c r="B33" s="1" t="s">
+        <x:v>305</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:5">
-      <x:c r="E34" s="7" t="s">
+      <x:c r="C34" s="1" t="s">
+        <x:v>306</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:5">
+      <x:c r="D35" s="1" t="s">
+        <x:v>307</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:5">
+      <x:c r="E36" s="7" t="s">
         <x:v>66</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:5">
-      <x:c r="B35" s="1" t="s">
-        <x:v>296</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:5">
-      <x:c r="C36" s="7" t="s">
-        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:5">
       <x:c r="B37" s="1" t="s">
-        <x:v>297</x:v>
+        <x:v>308</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:5">
       <x:c r="C38" s="7" t="s">
-        <x:v>41</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:5">
       <x:c r="B39" s="1" t="s">
-        <x:v>298</x:v>
+        <x:v>309</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:5">
       <x:c r="C40" s="7" t="s">
-        <x:v>11</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:5">
       <x:c r="B41" s="1" t="s">
-        <x:v>299</x:v>
+        <x:v>310</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:5">
       <x:c r="C42" s="7" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:5">
+      <x:c r="B43" s="1" t="s">
+        <x:v>311</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:5">
+      <x:c r="C44" s="7" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -1689,15 +1738,16 @@
     <x:hyperlink ref="C18" location="'SHOWTHEUSEOFBACKGROUND'!A1" display="Show the use of background"/>
     <x:hyperlink ref="C20" location="'SHOWINGTABLEUSAGE'!A1" display="Showing table usage"/>
     <x:hyperlink ref="C22" location="'SHOWTHECOMPARETOFEATURE'!A1" display="Show the compare to feature"/>
-    <x:hyperlink ref="C24" location="'ATTRIBUTEOVERLOADING'!A1" display="Attribute overloading"/>
-    <x:hyperlink ref="C26" location="'CALLINGSTEPSFROMSTEPDEFINITIONS'!A1" display="Calling Steps from StepDefinitions"/>
-    <x:hyperlink ref="C28" location="'STEPARGUMENTTRANSFORMATIONS'!A1" display="Step Argument Transformations"/>
-    <x:hyperlink ref="C30" location="'INJECTINGCONTEXTINTOSTEPSPECIFI'!A1" display="Injecting context into step specifications"/>
-    <x:hyperlink ref="E34" location="'NESTEDFOLDEREXAMPLE'!A1" display="Nested Folder Example"/>
-    <x:hyperlink ref="C36" location="'MULTILINEFEATUREEXAMPLE'!A1" display="Multiline Feature Example"/>
-    <x:hyperlink ref="C38" location="'SAMPLEMARKDOWNFEATURE'!A1" display="Sample Markdown Feature"/>
-    <x:hyperlink ref="C40" location="'INTERACTIVEDHTMLVIEW'!A1" display="Interactive DHTML View"/>
-    <x:hyperlink ref="C42" location="'CLEARINGSCREEN'!A1" display="Clearing Screen"/>
+    <x:hyperlink ref="C24" location="'SUMMERING'!A1" display="Summering"/>
+    <x:hyperlink ref="C26" location="'ATTRIBUTEOVERLOADING'!A1" display="Attribute overloading"/>
+    <x:hyperlink ref="C28" location="'CALLINGSTEPSFROMSTEPDEFINITIONS'!A1" display="Calling Steps from StepDefinitions"/>
+    <x:hyperlink ref="C30" location="'STEPARGUMENTTRANSFORMATIONS'!A1" display="Step Argument Transformations"/>
+    <x:hyperlink ref="C32" location="'INJECTINGCONTEXTINTOSTEPSPECIFI'!A1" display="Injecting context into step specifications"/>
+    <x:hyperlink ref="E36" location="'NESTEDFOLDEREXAMPLE'!A1" display="Nested Folder Example"/>
+    <x:hyperlink ref="C38" location="'MULTILINEFEATUREEXAMPLE'!A1" display="Multiline Feature Example"/>
+    <x:hyperlink ref="C40" location="'SAMPLEMARKDOWNFEATURE'!A1" display="Sample Markdown Feature"/>
+    <x:hyperlink ref="C42" location="'INTERACTIVEDHTMLVIEW'!A1" display="Interactive DHTML View"/>
+    <x:hyperlink ref="C44" location="'CLEARINGSCREEN'!A1" display="Clearing Screen"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1712,7 +1762,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E31"/>
+  <x:dimension ref="A1:E18"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1720,17 +1770,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="1" t="s">
-        <x:v>188</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="B2" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="B4" s="1" t="s">
-        <x:v>190</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
@@ -1741,7 +1791,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
@@ -1749,12 +1799,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="B9" s="1" t="s">
-        <x:v>193</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
@@ -1765,7 +1815,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
@@ -1773,111 +1823,55 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="D13" s="3" t="s">
-        <x:v>119</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="E13" s="3" t="s">
-        <x:v>120</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="D14" s="4" t="s">
-        <x:v>179</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="E14" s="4" t="s">
-        <x:v>180</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="D15" s="4" t="s">
-        <x:v>181</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="E15" s="4" t="s">
+        <x:v>182</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5">
+      <x:c r="D16" s="4" t="s">
         <x:v>193</x:v>
       </x:c>
+      <x:c r="E16" s="4" t="s">
+        <x:v>194</x:v>
+      </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
-      <x:c r="B17" s="1" t="s">
+      <x:c r="D17" s="4" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="E17" s="4" t="s">
         <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
-      <x:c r="C18" s="0" t="s"/>
-    </x:row>
-    <x:row r="19" spans="1:5">
-      <x:c r="C19" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
+      <x:c r="D18" s="4" t="s">
         <x:v>197</x:v>
       </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5">
-      <x:c r="C20" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
+      <x:c r="E18" s="4" t="s">
         <x:v>198</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:5">
-      <x:c r="C21" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>199</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:5">
-      <x:c r="C22" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>200</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:5">
-      <x:c r="B24" s="1" t="s">
-        <x:v>201</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:5">
-      <x:c r="C25" s="0" t="s"/>
-    </x:row>
-    <x:row r="26" spans="1:5">
-      <x:c r="C26" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>202</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:5">
-      <x:c r="B28" s="1" t="s">
-        <x:v>203</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:5">
-      <x:c r="C29" s="0" t="s"/>
-    </x:row>
-    <x:row r="30" spans="1:5">
-      <x:c r="C30" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D30" s="0" t="s">
-        <x:v>204</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:5">
-      <x:c r="C31" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D31" s="0" t="s">
-        <x:v>205</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1894,188 +1888,172 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D33"/>
+  <x:dimension ref="A1:E31"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="1" t="s">
+        <x:v>199</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5">
+      <x:c r="B2" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="B4" s="1" t="s">
+        <x:v>201</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="C5" s="0" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="C6" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="C7" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5">
+      <x:c r="B9" s="1" t="s">
+        <x:v>204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5">
+      <x:c r="C10" s="0" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:5">
+      <x:c r="C11" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:5">
+      <x:c r="C12" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
         <x:v>206</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="B2" s="0" t="s">
+    <x:row r="13" spans="1:5">
+      <x:c r="D13" s="3" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="E13" s="3" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:5">
+      <x:c r="D14" s="4" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="E14" s="4" t="s">
+        <x:v>191</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:5">
+      <x:c r="D15" s="4" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="E15" s="4" t="s">
+        <x:v>204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:5">
+      <x:c r="B17" s="1" t="s">
         <x:v>207</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="B4" s="1" t="s">
-        <x:v>208</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="C5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:4">
-      <x:c r="C6" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>209</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4">
-      <x:c r="C7" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>210</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:4">
-      <x:c r="C8" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>211</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:4">
-      <x:c r="C9" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:4">
-      <x:c r="B11" s="1" t="s">
-        <x:v>213</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:4">
-      <x:c r="C12" s="0" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:4">
-      <x:c r="C13" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>214</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:4">
-      <x:c r="C14" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>210</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:4">
-      <x:c r="C15" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>215</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:4">
-      <x:c r="B17" s="1" t="s">
-        <x:v>216</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:4">
+    <x:row r="18" spans="1:5">
       <x:c r="C18" s="0" t="s"/>
     </x:row>
-    <x:row r="19" spans="1:4">
+    <x:row r="19" spans="1:5">
       <x:c r="C19" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>217</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:4">
+        <x:v>208</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:5">
       <x:c r="C20" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:5">
+      <x:c r="C21" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D20" s="0" t="s">
+      <x:c r="D21" s="0" t="s">
         <x:v>210</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:4">
-      <x:c r="C21" s="2" t="s">
+    <x:row r="22" spans="1:5">
+      <x:c r="C22" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>218</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:4">
-      <x:c r="B23" s="1" t="s">
-        <x:v>219</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:4">
-      <x:c r="C24" s="0" t="s"/>
-    </x:row>
-    <x:row r="25" spans="1:4">
-      <x:c r="C25" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>220</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:4">
+      <x:c r="D22" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:5">
+      <x:c r="B24" s="1" t="s">
+        <x:v>212</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:5">
+      <x:c r="C25" s="0" t="s"/>
+    </x:row>
+    <x:row r="26" spans="1:5">
       <x:c r="C26" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>210</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:4">
-      <x:c r="C27" s="2" t="s">
+        <x:v>213</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:5">
+      <x:c r="B28" s="1" t="s">
+        <x:v>214</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:5">
+      <x:c r="C29" s="0" t="s"/>
+    </x:row>
+    <x:row r="30" spans="1:5">
+      <x:c r="C30" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:5">
+      <x:c r="C31" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>221</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:4">
-      <x:c r="B29" s="1" t="s">
-        <x:v>222</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:4">
-      <x:c r="C30" s="0" t="s"/>
-    </x:row>
-    <x:row r="31" spans="1:4">
-      <x:c r="C31" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>223</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:4">
-      <x:c r="C32" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D32" s="0" t="s">
-        <x:v>210</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:4">
-      <x:c r="C33" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D33" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2092,7 +2070,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D27"/>
+  <x:dimension ref="A1:D33"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -2100,17 +2078,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>225</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>218</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>227</x:v>
+        <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2121,103 +2099,119 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="C7" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="C8" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>229</x:v>
+      <x:c r="D8" s="0" t="s">
+        <x:v>222</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
-      <x:c r="B9" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:4">
-      <x:c r="C10" s="0" t="s"/>
+      <x:c r="C9" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
-      <x:c r="C11" s="2" t="s">
+      <x:c r="B11" s="1" t="s">
+        <x:v>224</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="C12" s="0" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="C13" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
+      <x:c r="D13" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="C14" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="C15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="B17" s="1" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="C18" s="0" t="s"/>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="C19" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
         <x:v>228</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:4">
-      <x:c r="C12" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>231</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:4">
-      <x:c r="B14" s="1" t="s">
-        <x:v>232</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:4">
-      <x:c r="C15" s="0" t="s"/>
-    </x:row>
-    <x:row r="16" spans="1:4">
-      <x:c r="C16" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>228</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:4">
-      <x:c r="C17" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>233</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:4">
-      <x:c r="B19" s="1" t="s">
-        <x:v>234</x:v>
-      </x:c>
-    </x:row>
     <x:row r="20" spans="1:4">
-      <x:c r="C20" s="0" t="s"/>
+      <x:c r="C20" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="C21" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="B23" s="1" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="C24" s="0" t="s"/>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="C25" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>228</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:4">
-      <x:c r="C22" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>235</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:4">
-      <x:c r="B24" s="1" t="s">
-        <x:v>236</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:4">
-      <x:c r="C25" s="0" t="s"/>
+      <x:c r="D25" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
       <x:c r="C26" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>221</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:4">
@@ -2225,7 +2219,39 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="B29" s="1" t="s">
+        <x:v>233</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="C30" s="0" t="s"/>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="C31" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="C32" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="C33" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>235</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2242,7 +2268,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D8"/>
+  <x:dimension ref="A1:D27"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -2250,17 +2276,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>238</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>237</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>240</x:v>
+        <x:v>238</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2271,23 +2297,111 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>241</x:v>
+        <x:v>239</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="C7" s="2" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="B9" s="1" t="s">
+        <x:v>241</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="C10" s="0" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="C11" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="C12" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
         <x:v>242</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4">
-      <x:c r="C8" s="2" t="s">
+    <x:row r="14" spans="1:4">
+      <x:c r="B14" s="1" t="s">
+        <x:v>243</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="C15" s="0" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="C16" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="C17" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>243</x:v>
+      <x:c r="D17" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="B19" s="1" t="s">
+        <x:v>245</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="C20" s="0" t="s"/>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="C21" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="C22" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>246</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="B24" s="1" t="s">
+        <x:v>247</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="C25" s="0" t="s"/>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="C26" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="C27" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>248</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2304,7 +2418,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D17"/>
+  <x:dimension ref="A1:D8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -2312,17 +2426,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>244</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>245</x:v>
+        <x:v>250</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>246</x:v>
+        <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2333,7 +2447,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>247</x:v>
+        <x:v>252</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -2341,7 +2455,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -2349,63 +2463,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>249</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:4">
-      <x:c r="B10" s="1" t="s">
-        <x:v>250</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:4">
-      <x:c r="C11" s="0" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:4">
-      <x:c r="C12" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>247</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:4">
-      <x:c r="C13" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>251</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:4">
-      <x:c r="C14" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>248</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:4">
-      <x:c r="C15" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>249</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:4">
-      <x:c r="C16" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>252</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:4">
-      <x:c r="C17" s="2" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2422,7 +2480,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D20"/>
+  <x:dimension ref="A1:D17"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -2430,17 +2488,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2451,7 +2509,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -2459,7 +2517,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -2467,12 +2525,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="B10" s="1" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -2483,12 +2541,12 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>258</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="C13" s="2" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>262</x:v>
@@ -2496,42 +2554,34 @@
     </x:row>
     <x:row r="14" spans="1:4">
       <x:c r="C14" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>259</x:v>
       </x:c>
     </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="C15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
     <x:row r="16" spans="1:4">
-      <x:c r="B16" s="1" t="s">
+      <x:c r="C16" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
         <x:v>263</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
-      <x:c r="C17" s="0" t="s"/>
-    </x:row>
-    <x:row r="18" spans="1:4">
-      <x:c r="C18" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
+      <x:c r="C17" s="2" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
         <x:v>264</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:4">
-      <x:c r="C19" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>265</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:4">
-      <x:c r="C20" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>259</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2548,6 +2598,132 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
+  <x:dimension ref="A1:D20"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="1" t="s">
+        <x:v>265</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="B2" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="B4" s="1" t="s">
+        <x:v>267</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="C5" s="0" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="C6" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>268</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="C7" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="C8" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="B10" s="1" t="s">
+        <x:v>271</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="C11" s="0" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="C12" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="C13" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="C14" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="B16" s="1" t="s">
+        <x:v>274</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="C17" s="0" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="C18" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="C19" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="C20" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
   <x:dimension ref="A1:D30"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -2556,17 +2732,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>266</x:v>
+        <x:v>277</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>268</x:v>
+        <x:v>279</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2606,7 +2782,7 @@
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="B11" s="1" t="s">
-        <x:v>269</x:v>
+        <x:v>280</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -2633,7 +2809,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>281</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -2641,12 +2817,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>282</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="B18" s="1" t="s">
-        <x:v>272</x:v>
+        <x:v>283</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -2673,7 +2849,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>273</x:v>
+        <x:v>284</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
@@ -2681,12 +2857,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>274</x:v>
+        <x:v>285</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="B25" s="1" t="s">
-        <x:v>275</x:v>
+        <x:v>286</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
@@ -2705,7 +2881,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>287</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
@@ -2713,7 +2889,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>277</x:v>
+        <x:v>288</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4">
@@ -2721,7 +2897,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>278</x:v>
+        <x:v>289</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3731,333 +3907,60 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F41"/>
+  <x:dimension ref="A1:D9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
         <x:v>115</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
+    <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
         <x:v>116</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:6">
+    <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
         <x:v>117</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:6">
+    <x:row r="5" spans="1:4">
       <x:c r="C5" s="0" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:6">
+    <x:row r="6" spans="1:4">
       <x:c r="C6" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>118</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:6">
-      <x:c r="D7" s="3" t="s">
         <x:v>119</x:v>
       </x:c>
-      <x:c r="E7" s="3" t="s">
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="C7" s="2" t="s">
         <x:v>120</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6">
-      <x:c r="D8" s="4" t="s">
+      <x:c r="D7" s="0" t="s">
         <x:v>121</x:v>
       </x:c>
-      <x:c r="E8" s="4" t="s">
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="C8" s="2" t="s">
         <x:v>122</x:v>
       </x:c>
-    </x:row>
-    <x:row r="9" spans="1:6">
-      <x:c r="D9" s="4" t="s">
+      <x:c r="D8" s="0" t="s">
         <x:v>123</x:v>
       </x:c>
-      <x:c r="E9" s="4" t="s">
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="C9" s="2" t="s">
         <x:v>124</x:v>
       </x:c>
-    </x:row>
-    <x:row r="10" spans="1:6">
-      <x:c r="D10" s="4" t="s">
+      <x:c r="D9" s="0" t="s">
         <x:v>125</x:v>
-      </x:c>
-      <x:c r="E10" s="6">
-        <x:v>26581</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:6">
-      <x:c r="C11" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>126</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:6">
-      <x:c r="D12" s="3" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="E12" s="3" t="s">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:6">
-      <x:c r="D13" s="4" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E13" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:6">
-      <x:c r="D14" s="4" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="E14" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:6">
-      <x:c r="D15" s="4" t="s">
-        <x:v>127</x:v>
-      </x:c>
-      <x:c r="E15" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:6">
-      <x:c r="C16" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>126</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:6">
-      <x:c r="D17" s="3" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="E17" s="3" t="s">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:6">
-      <x:c r="D18" s="4" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E18" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:6">
-      <x:c r="D19" s="4" t="s">
-        <x:v>127</x:v>
-      </x:c>
-      <x:c r="E19" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:6">
-      <x:c r="C20" s="2" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>128</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:6">
-      <x:c r="D21" s="3" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="E21" s="3" t="s">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:6">
-      <x:c r="D22" s="4" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E22" s="4" t="s">
-        <x:v>129</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:6">
-      <x:c r="D23" s="4" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="E23" s="4" t="s">
-        <x:v>130</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:6">
-      <x:c r="D24" s="4" t="s">
-        <x:v>127</x:v>
-      </x:c>
-      <x:c r="E24" s="6">
-        <x:v>27282</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:6">
-      <x:c r="B26" s="1" t="s">
-        <x:v>131</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:6">
-      <x:c r="C27" s="0" t="s"/>
-    </x:row>
-    <x:row r="28" spans="1:6">
-      <x:c r="C28" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>132</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:6">
-      <x:c r="D29" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E29" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F29" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:6">
-      <x:c r="D30" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="E30" s="4" t="s">
-        <x:v>133</x:v>
-      </x:c>
-      <x:c r="F30" s="6">
-        <x:v>26581</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:6">
-      <x:c r="D31" s="4" t="s">
-        <x:v>129</x:v>
-      </x:c>
-      <x:c r="E31" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="F31" s="6">
-        <x:v>28126</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:6">
-      <x:c r="D32" s="4" t="s">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="E32" s="4" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="F32" s="6">
-        <x:v>27123</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:6">
-      <x:c r="C33" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D33" s="0" t="s">
-        <x:v>136</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:6">
-      <x:c r="D34" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E34" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F34" s="3" t="s">
-        <x:v>127</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:6">
-      <x:c r="D35" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="E35" s="4" t="s">
-        <x:v>133</x:v>
-      </x:c>
-      <x:c r="F35" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:6">
-      <x:c r="D36" s="4" t="s">
-        <x:v>129</x:v>
-      </x:c>
-      <x:c r="E36" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="F36" s="6">
-        <x:v>28126</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:6">
-      <x:c r="D37" s="4" t="s">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="E37" s="4" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="F37" s="6">
-        <x:v>27123</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:6">
-      <x:c r="C38" s="2" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="D38" s="0" t="s">
-        <x:v>137</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="1:6">
-      <x:c r="D39" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E39" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F39" s="3" t="s">
-        <x:v>127</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:6">
-      <x:c r="D40" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="E40" s="4" t="s">
-        <x:v>133</x:v>
-      </x:c>
-      <x:c r="F40" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:6">
-      <x:c r="D41" s="4" t="s">
-        <x:v>129</x:v>
-      </x:c>
-      <x:c r="E41" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="F41" s="6">
-        <x:v>28126</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -4074,556 +3977,333 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AI44"/>
+  <x:dimension ref="A1:F41"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:35">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="1" t="s">
-        <x:v>138</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:35">
+        <x:v>126</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
       <x:c r="B2" s="0" t="s">
-        <x:v>139</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:35">
+        <x:v>127</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
       <x:c r="B4" s="1" t="s">
-        <x:v>140</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:35">
+        <x:v>128</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
       <x:c r="C5" s="0" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:35">
+    <x:row r="6" spans="1:6">
       <x:c r="C6" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>141</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:35">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
       <x:c r="D7" s="3" t="s">
-        <x:v>121</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="E7" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F7" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="G7" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:35">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
       <x:c r="D8" s="4" t="s">
-        <x:v>122</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="E8" s="4" t="s">
         <x:v>133</x:v>
       </x:c>
-      <x:c r="F8" s="6">
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="D9" s="4" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="E9" s="4" t="s">
+        <x:v>135</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="D10" s="4" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="E10" s="6">
         <x:v>26581</x:v>
       </x:c>
-      <x:c r="G8" s="4" t="n">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:35">
-      <x:c r="D9" s="4" t="s">
-        <x:v>129</x:v>
-      </x:c>
-      <x:c r="E9" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="F9" s="6">
-        <x:v>28126</x:v>
-      </x:c>
-      <x:c r="G9" s="4" t="n">
-        <x:v>500</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:35">
-      <x:c r="D10" s="4" t="s">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="E10" s="4" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="F10" s="6">
-        <x:v>27123</x:v>
-      </x:c>
-      <x:c r="G10" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:35">
+    </x:row>
+    <x:row r="11" spans="1:6">
       <x:c r="C11" s="2" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>143</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:35">
-      <x:c r="C12" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>144</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:35">
-      <x:c r="D13" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E13" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F13" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="G13" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:35">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="D12" s="3" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="E12" s="3" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="D13" s="4" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E13" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
       <x:c r="D14" s="4" t="s">
         <x:v>134</x:v>
       </x:c>
       <x:c r="E14" s="4" t="s">
         <x:v>135</x:v>
       </x:c>
-      <x:c r="F14" s="6">
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="D15" s="4" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="E15" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="C16" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="D17" s="3" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="E17" s="3" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="D18" s="4" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E18" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="D19" s="4" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="E19" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="C20" s="2" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="D21" s="3" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="E21" s="3" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="D22" s="4" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E22" s="4" t="s">
+        <x:v>140</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="D23" s="4" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="E23" s="4" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="D24" s="4" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="E24" s="6">
+        <x:v>27282</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="B26" s="1" t="s">
+        <x:v>142</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="C27" s="0" t="s"/>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="C28" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="D29" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E29" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F29" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="D30" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E30" s="4" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="F30" s="6">
+        <x:v>26581</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="D31" s="4" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E31" s="4" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="F31" s="6">
+        <x:v>28126</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="D32" s="4" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="E32" s="4" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="F32" s="6">
         <x:v>27123</x:v>
       </x:c>
-      <x:c r="G14" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:35">
-      <x:c r="B16" s="1" t="s">
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="C33" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="D34" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E34" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F34" s="3" t="s">
+        <x:v>138</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="D35" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E35" s="4" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="F35" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="D36" s="4" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E36" s="4" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="F36" s="6">
+        <x:v>28126</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="D37" s="4" t="s">
         <x:v>145</x:v>
       </x:c>
-    </x:row>
-    <x:row r="17" spans="1:35">
-      <x:c r="C17" s="0" t="s"/>
-    </x:row>
-    <x:row r="18" spans="1:35">
-      <x:c r="C18" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
+      <x:c r="E37" s="4" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="F37" s="6">
+        <x:v>27123</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="C38" s="2" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="D39" s="3" t="s">
         <x:v>132</x:v>
       </x:c>
-    </x:row>
-    <x:row r="19" spans="1:35">
-      <x:c r="D19" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E19" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F19" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="G19" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:35">
-      <x:c r="D20" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="E20" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="F20" s="6">
-        <x:v>26581</x:v>
-      </x:c>
-      <x:c r="G20" s="4" t="n">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:35">
-      <x:c r="D21" s="4" t="s">
-        <x:v>129</x:v>
-      </x:c>
-      <x:c r="E21" s="4" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="F21" s="6">
+      <x:c r="E39" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F39" s="3" t="s">
+        <x:v>138</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="D40" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E40" s="4" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="F40" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="D41" s="4" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E41" s="4" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="F41" s="6">
         <x:v>28126</x:v>
-      </x:c>
-      <x:c r="G21" s="4" t="n">
-        <x:v>500</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:35">
-      <x:c r="D22" s="4" t="s">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="E22" s="4" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="F22" s="6">
-        <x:v>27123</x:v>
-      </x:c>
-      <x:c r="G22" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:35">
-      <x:c r="C23" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D23" s="0" t="s">
-        <x:v>143</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:35">
-      <x:c r="C24" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>147</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:35">
-      <x:c r="D25" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E25" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F25" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="G25" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:35">
-      <x:c r="D26" s="4" t="s">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="E26" s="4" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="F26" s="6">
-        <x:v>27123</x:v>
-      </x:c>
-      <x:c r="G26" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:35">
-      <x:c r="B28" s="1" t="s">
-        <x:v>148</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:35">
-      <x:c r="C29" s="0" t="s"/>
-    </x:row>
-    <x:row r="30" spans="1:35">
-      <x:c r="C30" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D30" s="0" t="s">
-        <x:v>149</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:35">
-      <x:c r="D31" s="3" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="E31" s="3" t="s">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:35">
-      <x:c r="D32" s="4" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E32" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:35">
-      <x:c r="D33" s="4" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="E33" s="4" t="s">
-        <x:v>130</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:35">
-      <x:c r="D34" s="4" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="E34" s="6">
-        <x:v>26581</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:35">
-      <x:c r="D35" s="4" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="E35" s="4" t="n">
-        <x:v>100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:35">
-      <x:c r="C36" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D36" s="0" t="s">
-        <x:v>147</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:35">
-      <x:c r="D37" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E37" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F37" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="G37" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:35">
-      <x:c r="D38" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="E38" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="F38" s="6">
-        <x:v>26581</x:v>
-      </x:c>
-      <x:c r="G38" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:35">
-      <x:c r="B40" s="1" t="s">
-        <x:v>150</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:35">
-      <x:c r="C41" s="0" t="s"/>
-    </x:row>
-    <x:row r="42" spans="1:35">
-      <x:c r="C42" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D42" s="0" t="s">
-        <x:v>151</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:35">
-      <x:c r="D43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="E43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="F43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="G43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="H43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="I43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="J43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="K43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="L43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="M43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="N43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="O43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="P43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="Q43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="R43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="S43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="T43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="U43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="V43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="W43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="X43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="Y43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="Z43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="AA43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="AB43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="AC43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="AD43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="AE43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="AF43" s="3" t="s">
-        <x:v>121</x:v>
-      </x:c>
-      <x:c r="AG43" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="AH43" s="3" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="AI43" s="3" t="s">
-        <x:v>142</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44" spans="1:35">
-      <x:c r="D44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="E44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="F44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="G44" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="H44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="I44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="J44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="K44" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="L44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="M44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="N44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="O44" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="P44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="Q44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="R44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="S44" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="T44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="U44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="V44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="W44" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="X44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="Y44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="Z44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="AA44" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="AB44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="AC44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="AD44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="AE44" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="AF44" s="4" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="AG44" s="4" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="AH44" s="6">
-        <x:v>26552</x:v>
-      </x:c>
-      <x:c r="AI44" s="4" t="n">
-        <x:v>1000</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -4640,68 +4320,556 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D12"/>
+  <x:dimension ref="A1:AI44"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:35">
       <x:c r="A1" s="1" t="s">
+        <x:v>149</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:35">
+      <x:c r="B2" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:35">
+      <x:c r="B4" s="1" t="s">
+        <x:v>151</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:35">
+      <x:c r="C5" s="0" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:35">
+      <x:c r="C6" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
         <x:v>152</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="B2" s="0" t="s">
+    <x:row r="7" spans="1:35">
+      <x:c r="D7" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E7" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F7" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="G7" s="3" t="s">
         <x:v>153</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="B4" s="1" t="s">
-        <x:v>154</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="C5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:4">
-      <x:c r="C6" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>155</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4">
-      <x:c r="C7" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>156</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:4">
-      <x:c r="B9" s="1" t="s">
-        <x:v>157</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:4">
-      <x:c r="C10" s="0" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:4">
+    <x:row r="8" spans="1:35">
+      <x:c r="D8" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E8" s="4" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="F8" s="6">
+        <x:v>26581</x:v>
+      </x:c>
+      <x:c r="G8" s="4" t="n">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:35">
+      <x:c r="D9" s="4" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E9" s="4" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="F9" s="6">
+        <x:v>28126</x:v>
+      </x:c>
+      <x:c r="G9" s="4" t="n">
+        <x:v>500</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:35">
+      <x:c r="D10" s="4" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="E10" s="4" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="F10" s="6">
+        <x:v>27123</x:v>
+      </x:c>
+      <x:c r="G10" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:35">
       <x:c r="C11" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>158</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:4">
+        <x:v>154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:35">
       <x:c r="C12" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:35">
+      <x:c r="D13" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E13" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F13" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="G13" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:35">
+      <x:c r="D14" s="4" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="E14" s="4" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="F14" s="6">
+        <x:v>27123</x:v>
+      </x:c>
+      <x:c r="G14" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:35">
+      <x:c r="B16" s="1" t="s">
+        <x:v>156</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:35">
+      <x:c r="C17" s="0" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:35">
+      <x:c r="C18" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:35">
+      <x:c r="D19" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E19" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F19" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="G19" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:35">
+      <x:c r="D20" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E20" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="F20" s="6">
+        <x:v>26581</x:v>
+      </x:c>
+      <x:c r="G20" s="4" t="n">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:35">
+      <x:c r="D21" s="4" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E21" s="4" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="F21" s="6">
+        <x:v>28126</x:v>
+      </x:c>
+      <x:c r="G21" s="4" t="n">
+        <x:v>500</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:35">
+      <x:c r="D22" s="4" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="E22" s="4" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="F22" s="6">
+        <x:v>27123</x:v>
+      </x:c>
+      <x:c r="G22" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:35">
+      <x:c r="C23" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:35">
+      <x:c r="C24" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:35">
+      <x:c r="D25" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E25" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F25" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="G25" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:35">
+      <x:c r="D26" s="4" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="E26" s="4" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="F26" s="6">
+        <x:v>27123</x:v>
+      </x:c>
+      <x:c r="G26" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:35">
+      <x:c r="B28" s="1" t="s">
         <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:35">
+      <x:c r="C29" s="0" t="s"/>
+    </x:row>
+    <x:row r="30" spans="1:35">
+      <x:c r="C30" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:35">
+      <x:c r="D31" s="3" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="E31" s="3" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:35">
+      <x:c r="D32" s="4" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E32" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:35">
+      <x:c r="D33" s="4" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="E33" s="4" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:35">
+      <x:c r="D34" s="4" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="E34" s="6">
+        <x:v>26581</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:35">
+      <x:c r="D35" s="4" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="E35" s="4" t="n">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:35">
+      <x:c r="C36" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:35">
+      <x:c r="D37" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E37" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F37" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="G37" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:35">
+      <x:c r="D38" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E38" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="F38" s="6">
+        <x:v>26581</x:v>
+      </x:c>
+      <x:c r="G38" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:35">
+      <x:c r="B40" s="1" t="s">
+        <x:v>161</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:35">
+      <x:c r="C41" s="0" t="s"/>
+    </x:row>
+    <x:row r="42" spans="1:35">
+      <x:c r="C42" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:35">
+      <x:c r="D43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="F43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="G43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="H43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="I43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="J43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="K43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="L43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="M43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="N43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="O43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="P43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="Q43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="R43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="S43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="T43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="U43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="V43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="W43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="X43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="Y43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="Z43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="AA43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="AB43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="AC43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="AD43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="AE43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="AF43" s="3" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="AG43" s="3" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="AH43" s="3" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="AI43" s="3" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:35">
+      <x:c r="D44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="F44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="G44" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="H44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="I44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="J44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="K44" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="L44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="M44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="N44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="O44" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="P44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="Q44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="R44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="S44" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="T44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="U44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="V44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="W44" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="X44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="Y44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="Z44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="AA44" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="AB44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="AC44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="AD44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="AE44" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="AF44" s="4" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="AG44" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="AH44" s="6">
+        <x:v>26552</x:v>
+      </x:c>
+      <x:c r="AI44" s="4" t="n">
+        <x:v>1000</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -4718,278 +4886,68 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F36"/>
+  <x:dimension ref="A1:D12"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>160</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:6">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6">
-      <x:c r="B4" s="0" t="s">
-        <x:v>162</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:6">
+        <x:v>164</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="B4" s="1" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
       <x:c r="C5" s="0" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:6">
+    <x:row r="6" spans="1:4">
       <x:c r="C6" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>163</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:6">
+        <x:v>166</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
       <x:c r="C7" s="2" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>164</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6">
-      <x:c r="C8" s="2" t="s">
+        <x:v>167</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="B9" s="1" t="s">
+        <x:v>168</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="C10" s="0" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="C11" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>165</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:6">
-      <x:c r="C9" s="2" t="s">
+      <x:c r="D11" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="C12" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:6">
-      <x:c r="B11" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:6">
-      <x:c r="C12" s="0" t="s"/>
-      <x:c r="D12" s="3" t="s">
-        <x:v>167</x:v>
-      </x:c>
-      <x:c r="E12" s="3" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="F12" s="3" t="s">
-        <x:v>169</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:6">
-      <x:c r="D13" s="4" t="n">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E13" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F13" s="4" t="n">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:6">
-      <x:c r="D14" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E14" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F14" s="4" t="n">
-        <x:v>40</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:6">
-      <x:c r="D15" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E15" s="4" t="n">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F15" s="4" t="n">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:6">
-      <x:c r="B16" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:6">
-      <x:c r="C17" s="0" t="s"/>
-      <x:c r="D17" s="3" t="s">
-        <x:v>167</x:v>
-      </x:c>
-      <x:c r="E17" s="3" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="F17" s="3" t="s">
-        <x:v>169</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:6">
-      <x:c r="D18" s="4" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="E18" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F18" s="4" t="n">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:6">
-      <x:c r="D19" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="E19" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F19" s="4" t="n">
-        <x:v>1020</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:6">
-      <x:c r="B21" s="0" t="s">
+      <x:c r="D12" s="0" t="s">
         <x:v>170</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:6">
-      <x:c r="C22" s="0" t="s"/>
-    </x:row>
-    <x:row r="23" spans="1:6">
-      <x:c r="C23" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D23" s="0" t="s">
-        <x:v>163</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:6">
-      <x:c r="C24" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>164</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:6">
-      <x:c r="C25" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>165</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:6">
-      <x:c r="C26" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:6">
-      <x:c r="B28" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:6">
-      <x:c r="C29" s="0" t="s"/>
-      <x:c r="D29" s="3" t="s">
-        <x:v>167</x:v>
-      </x:c>
-      <x:c r="E29" s="3" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="F29" s="3" t="s">
-        <x:v>169</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:6">
-      <x:c r="D30" s="4" t="n">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E30" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F30" s="4" t="n">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:6">
-      <x:c r="D31" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E31" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F31" s="4" t="n">
-        <x:v>40</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:6">
-      <x:c r="D32" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E32" s="4" t="n">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F32" s="4" t="n">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:6">
-      <x:c r="B33" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:6">
-      <x:c r="C34" s="0" t="s"/>
-      <x:c r="D34" s="3" t="s">
-        <x:v>167</x:v>
-      </x:c>
-      <x:c r="E34" s="3" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="F34" s="3" t="s">
-        <x:v>169</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:6">
-      <x:c r="D35" s="4" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="E35" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F35" s="4" t="n">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:6">
-      <x:c r="D36" s="4" t="n">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="E36" s="4" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F36" s="4" t="n">
-        <x:v>1020</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -5006,116 +4964,278 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E18"/>
+  <x:dimension ref="A1:F36"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="1" t="s">
         <x:v>171</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="B2" s="0" t="s">
         <x:v>172</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="B4" s="1" t="s">
+    <x:row r="4" spans="1:6">
+      <x:c r="B4" s="0" t="s">
         <x:v>173</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:5">
+    <x:row r="5" spans="1:6">
       <x:c r="C5" s="0" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:5">
+    <x:row r="6" spans="1:6">
       <x:c r="C6" s="2" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>174</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:5">
+    <x:row r="7" spans="1:6">
       <x:c r="C7" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>175</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="B9" s="1" t="s">
+    <x:row r="8" spans="1:6">
+      <x:c r="C8" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
         <x:v>176</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:5">
-      <x:c r="C10" s="0" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="C11" s="2" t="s">
+    <x:row r="9" spans="1:6">
+      <x:c r="C9" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="B11" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="C12" s="0" t="s"/>
+      <x:c r="D12" s="3" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="E12" s="3" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="F12" s="3" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="D13" s="4" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E13" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F13" s="4" t="n">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="D14" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E14" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F14" s="4" t="n">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="D15" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E15" s="4" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="F15" s="4" t="n">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="B16" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="C17" s="0" t="s"/>
+      <x:c r="D17" s="3" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="E17" s="3" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="F17" s="3" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="D18" s="4" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E18" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F18" s="4" t="n">
+        <x:v>120</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="D19" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="E19" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F19" s="4" t="n">
+        <x:v>1020</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="B21" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="C22" s="0" t="s"/>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="C23" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="C24" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="C25" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
+      <x:c r="D25" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="C26" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
         <x:v>177</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="C12" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
+    <x:row r="28" spans="1:6">
+      <x:c r="B28" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="C29" s="0" t="s"/>
+      <x:c r="D29" s="3" t="s">
         <x:v>178</x:v>
       </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
-      <x:c r="D13" s="3" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="E13" s="3" t="s">
+      <x:c r="E29" s="3" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="F29" s="3" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="D30" s="4" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E30" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F30" s="4" t="n">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="D31" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E31" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F31" s="4" t="n">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="D32" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E32" s="4" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="F32" s="4" t="n">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="B33" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="C34" s="0" t="s"/>
+      <x:c r="D34" s="3" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="E34" s="3" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="F34" s="3" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="D35" s="4" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E35" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F35" s="4" t="n">
         <x:v>120</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="D14" s="4" t="s">
-        <x:v>179</x:v>
-      </x:c>
-      <x:c r="E14" s="4" t="s">
-        <x:v>180</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5">
-      <x:c r="D15" s="4" t="s">
-        <x:v>181</x:v>
-      </x:c>
-      <x:c r="E15" s="4" t="s">
-        <x:v>171</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5">
-      <x:c r="D16" s="4" t="s">
-        <x:v>182</x:v>
-      </x:c>
-      <x:c r="E16" s="4" t="s">
-        <x:v>183</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5">
-      <x:c r="D17" s="4" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="E17" s="4" t="s">
-        <x:v>185</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5">
-      <x:c r="D18" s="4" t="s">
-        <x:v>186</x:v>
-      </x:c>
-      <x:c r="E18" s="4" t="s">
-        <x:v>187</x:v>
+    <x:row r="36" spans="1:6">
+      <x:c r="D36" s="4" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="E36" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F36" s="4" t="n">
+        <x:v>1020</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Output of version 1.0.1
</commit_message>
<xml_diff>
--- a/Output/Excel/features.xlsx
+++ b/Output/Excel/features.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="314">
   <x:si>
     <x:t>Clearing Screen</x:t>
   </x:si>
@@ -191,6 +191,15 @@
 Including a picture: ![](./image.png)</x:t>
   </x:si>
   <x:si>
+    <x:t>This is the *coolest* background</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have initialized the Sum-variable to 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I add 1 to the Sum-variable</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sample Markdown Scenario Example</x:t>
   </x:si>
   <x:si>
@@ -594,9 +603,6 @@
   </x:si>
   <x:si>
     <x:t>Add 1 to the sum</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I add 1 to the Sum-variable</x:t>
   </x:si>
   <x:si>
     <x:t>the total sum should be 2</x:t>
@@ -1506,197 +1512,197 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="1" t="s">
-        <x:v>290</x:v>
+        <x:v>292</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="B2" s="7" t="s">
-        <x:v>277</x:v>
+        <x:v>279</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="B3" s="7" t="s">
-        <x:v>265</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="B4" s="1" t="s">
-        <x:v>291</x:v>
+        <x:v>293</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="C5" s="7" t="s">
-        <x:v>255</x:v>
+        <x:v>257</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="B6" s="1" t="s">
-        <x:v>292</x:v>
+        <x:v>294</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="C7" s="7" t="s">
-        <x:v>249</x:v>
+        <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="B8" s="1" t="s">
-        <x:v>293</x:v>
+        <x:v>295</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="C9" s="7" t="s">
-        <x:v>236</x:v>
+        <x:v>238</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="C10" s="7" t="s">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="B11" s="1" t="s">
-        <x:v>294</x:v>
+        <x:v>296</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="C12" s="7" t="s">
-        <x:v>199</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="B13" s="1" t="s">
-        <x:v>295</x:v>
+        <x:v>297</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="C14" s="7" t="s">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="B15" s="1" t="s">
-        <x:v>296</x:v>
+        <x:v>298</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="C16" s="7" t="s">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="B17" s="1" t="s">
-        <x:v>297</x:v>
+        <x:v>299</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="C18" s="7" t="s">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
       <x:c r="B19" s="1" t="s">
-        <x:v>298</x:v>
+        <x:v>300</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="C20" s="7" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
       <x:c r="B21" s="1" t="s">
-        <x:v>299</x:v>
+        <x:v>301</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
       <x:c r="C22" s="7" t="s">
-        <x:v>126</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
       <x:c r="B23" s="1" t="s">
-        <x:v>300</x:v>
+        <x:v>302</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
       <x:c r="C24" s="7" t="s">
-        <x:v>115</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
       <x:c r="B25" s="1" t="s">
-        <x:v>301</x:v>
+        <x:v>303</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
       <x:c r="C26" s="7" t="s">
-        <x:v>104</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
       <x:c r="B27" s="1" t="s">
-        <x:v>302</x:v>
+        <x:v>304</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5">
       <x:c r="C28" s="7" t="s">
-        <x:v>93</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
       <x:c r="B29" s="1" t="s">
-        <x:v>303</x:v>
+        <x:v>305</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:5">
       <x:c r="C30" s="7" t="s">
-        <x:v>87</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
       <x:c r="B31" s="1" t="s">
-        <x:v>304</x:v>
+        <x:v>306</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:5">
       <x:c r="C32" s="7" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:5">
       <x:c r="B33" s="1" t="s">
-        <x:v>305</x:v>
+        <x:v>307</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:5">
       <x:c r="C34" s="1" t="s">
-        <x:v>306</x:v>
+        <x:v>308</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:5">
       <x:c r="D35" s="1" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:5">
       <x:c r="E36" s="7" t="s">
-        <x:v>66</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:5">
       <x:c r="B37" s="1" t="s">
-        <x:v>308</x:v>
+        <x:v>310</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:5">
       <x:c r="C38" s="7" t="s">
-        <x:v>57</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:5">
       <x:c r="B39" s="1" t="s">
-        <x:v>309</x:v>
+        <x:v>311</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:5">
@@ -1706,7 +1712,7 @@
     </x:row>
     <x:row r="41" spans="1:5">
       <x:c r="B41" s="1" t="s">
-        <x:v>310</x:v>
+        <x:v>312</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:5">
@@ -1716,7 +1722,7 @@
     </x:row>
     <x:row r="43" spans="1:5">
       <x:c r="B43" s="1" t="s">
-        <x:v>311</x:v>
+        <x:v>313</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:5">
@@ -1770,17 +1776,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="1" t="s">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="B2" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="B4" s="1" t="s">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
@@ -1791,7 +1797,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
@@ -1799,12 +1805,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="B9" s="1" t="s">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
@@ -1815,7 +1821,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
@@ -1823,55 +1829,55 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="D13" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E13" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="D14" s="4" t="s">
-        <x:v>190</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="E14" s="4" t="s">
-        <x:v>191</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="D15" s="4" t="s">
-        <x:v>192</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="E15" s="4" t="s">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="D16" s="4" t="s">
-        <x:v>193</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="E16" s="4" t="s">
-        <x:v>194</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="D17" s="4" t="s">
-        <x:v>195</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="E17" s="4" t="s">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="D18" s="4" t="s">
-        <x:v>197</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="E18" s="4" t="s">
-        <x:v>198</x:v>
+        <x:v>200</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1896,17 +1902,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="1" t="s">
-        <x:v>199</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="B2" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>202</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="B4" s="1" t="s">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
@@ -1917,7 +1923,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>204</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
@@ -1925,12 +1931,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>205</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="B9" s="1" t="s">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
@@ -1941,7 +1947,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>207</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
@@ -1949,36 +1955,36 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>208</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="D13" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E13" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="D14" s="4" t="s">
-        <x:v>190</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="E14" s="4" t="s">
-        <x:v>191</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="D15" s="4" t="s">
-        <x:v>192</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="E15" s="4" t="s">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="B17" s="1" t="s">
-        <x:v>207</x:v>
+        <x:v>209</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
@@ -1989,7 +1995,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>210</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
@@ -1997,7 +2003,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
@@ -2005,7 +2011,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>212</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
@@ -2013,12 +2019,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
       <x:c r="B24" s="1" t="s">
-        <x:v>212</x:v>
+        <x:v>214</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
@@ -2029,12 +2035,12 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5">
       <x:c r="B28" s="1" t="s">
-        <x:v>214</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
@@ -2045,7 +2051,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
@@ -2053,7 +2059,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>218</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2078,17 +2084,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>219</x:v>
+        <x:v>221</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2099,7 +2105,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>222</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -2107,7 +2113,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -2115,7 +2121,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>224</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -2123,12 +2129,12 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>225</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="B11" s="1" t="s">
-        <x:v>224</x:v>
+        <x:v>226</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -2139,7 +2145,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>227</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -2147,7 +2153,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -2155,12 +2161,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>228</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="B17" s="1" t="s">
-        <x:v>227</x:v>
+        <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -2171,7 +2177,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>230</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -2179,7 +2185,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -2187,12 +2193,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>231</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="B23" s="1" t="s">
-        <x:v>230</x:v>
+        <x:v>232</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:4">
@@ -2203,7 +2209,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>233</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
@@ -2211,7 +2217,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:4">
@@ -2219,12 +2225,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>234</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
       <x:c r="B29" s="1" t="s">
-        <x:v>233</x:v>
+        <x:v>235</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4">
@@ -2235,7 +2241,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:4">
@@ -2243,7 +2249,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D32" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:4">
@@ -2251,7 +2257,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>237</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2276,17 +2282,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>236</x:v>
+        <x:v>238</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>239</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>238</x:v>
+        <x:v>240</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2297,7 +2303,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -2305,12 +2311,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>240</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="B9" s="1" t="s">
-        <x:v>241</x:v>
+        <x:v>243</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -2321,7 +2327,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -2329,12 +2335,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>242</x:v>
+        <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
       <x:c r="B14" s="1" t="s">
-        <x:v>243</x:v>
+        <x:v>245</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -2345,7 +2351,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -2353,12 +2359,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="B19" s="1" t="s">
-        <x:v>245</x:v>
+        <x:v>247</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -2369,7 +2375,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -2377,12 +2383,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>246</x:v>
+        <x:v>248</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="B24" s="1" t="s">
-        <x:v>247</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
@@ -2393,7 +2399,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:4">
@@ -2401,7 +2407,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>250</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2426,17 +2432,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>249</x:v>
+        <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>250</x:v>
+        <x:v>252</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>251</x:v>
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2447,7 +2453,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>252</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -2455,7 +2461,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -2463,7 +2469,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>256</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2488,17 +2494,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>255</x:v>
+        <x:v>257</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>258</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>257</x:v>
+        <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2509,7 +2515,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -2517,7 +2523,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -2525,12 +2531,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>262</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="B10" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>263</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -2541,7 +2547,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -2549,7 +2555,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>262</x:v>
+        <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -2557,7 +2563,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -2565,7 +2571,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>262</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -2573,15 +2579,15 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>265</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="C17" s="2" t="s">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>266</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2606,17 +2612,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>265</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>268</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>267</x:v>
+        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2627,7 +2633,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>270</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -2635,7 +2641,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>271</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -2643,12 +2649,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>272</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="B10" s="1" t="s">
-        <x:v>271</x:v>
+        <x:v>273</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -2659,7 +2665,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>272</x:v>
+        <x:v>274</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -2667,7 +2673,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>273</x:v>
+        <x:v>275</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -2675,12 +2681,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>272</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
       <x:c r="B16" s="1" t="s">
-        <x:v>274</x:v>
+        <x:v>276</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -2691,7 +2697,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>275</x:v>
+        <x:v>277</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -2699,7 +2705,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -2707,7 +2713,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>272</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2732,17 +2738,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>277</x:v>
+        <x:v>279</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>278</x:v>
+        <x:v>280</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>279</x:v>
+        <x:v>281</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -2769,7 +2775,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -2777,12 +2783,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="B11" s="1" t="s">
-        <x:v>280</x:v>
+        <x:v>282</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -2809,7 +2815,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>281</x:v>
+        <x:v>283</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -2817,12 +2823,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>282</x:v>
+        <x:v>284</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="B18" s="1" t="s">
-        <x:v>283</x:v>
+        <x:v>285</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -2849,7 +2855,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>284</x:v>
+        <x:v>286</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
@@ -2857,12 +2863,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>285</x:v>
+        <x:v>287</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="B25" s="1" t="s">
-        <x:v>286</x:v>
+        <x:v>288</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
@@ -2881,7 +2887,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>287</x:v>
+        <x:v>289</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
@@ -2889,7 +2895,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>288</x:v>
+        <x:v>290</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4">
@@ -2897,7 +2903,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>289</x:v>
+        <x:v>291</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3230,7 +3236,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E16"/>
+  <x:dimension ref="A1:E21"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -3247,13 +3253,11 @@
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
-      <x:c r="B4" s="1" t="s">
+      <x:c r="B4" s="1" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="C5" s="0" t="s">
         <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="C5" s="5" t="s">
-        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
@@ -3261,25 +3265,25 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="C7" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5">
+      <x:c r="B9" s="1" t="s">
         <x:v>46</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="B9" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="C10" s="5" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
@@ -3287,7 +3291,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
@@ -3295,31 +3299,57 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="B14" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="C15" s="5" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5">
+      <x:c r="C16" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="D15" s="3" t="s">
+    </x:row>
+    <x:row r="17" spans="1:5">
+      <x:c r="C17" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="E15" s="3" t="s">
+    </x:row>
+    <x:row r="19" spans="1:5">
+      <x:c r="B19" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:5">
-      <x:c r="D16" s="4" t="s">
+    <x:row r="20" spans="1:5">
+      <x:c r="C20" s="5" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="E16" s="4" t="s">
+      <x:c r="D20" s="3" t="s">
         <x:v>56</x:v>
+      </x:c>
+      <x:c r="E20" s="3" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:5">
+      <x:c r="D21" s="4" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E21" s="4" t="s">
+        <x:v>59</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3344,17 +3374,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>57</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>59</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -3365,22 +3395,22 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="D7" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
       <x:c r="D8" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="D9" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -3388,7 +3418,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -3396,7 +3426,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3421,17 +3451,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>66</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -3458,7 +3488,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -3466,7 +3496,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3491,17 +3521,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>73</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -3512,7 +3542,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -3520,12 +3550,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="B9" s="1" t="s">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -3536,7 +3566,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -3544,12 +3574,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
       <x:c r="B14" s="1" t="s">
-        <x:v>79</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -3560,7 +3590,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -3568,12 +3598,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="B19" s="1" t="s">
-        <x:v>82</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -3584,7 +3614,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -3592,7 +3622,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
@@ -3600,12 +3630,12 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="B25" s="1" t="s">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
@@ -3616,7 +3646,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:4">
@@ -3624,7 +3654,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
@@ -3632,7 +3662,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3657,17 +3687,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>87</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>89</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -3678,7 +3708,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -3686,7 +3716,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -3694,7 +3724,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3719,17 +3749,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>93</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>95</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -3740,7 +3770,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -3748,7 +3778,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -3756,7 +3786,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -3764,12 +3794,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="B11" s="1" t="s">
-        <x:v>100</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -3780,7 +3810,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -3788,7 +3818,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -3796,7 +3826,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3821,17 +3851,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>104</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>106</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -3842,7 +3872,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
@@ -3850,7 +3880,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
@@ -3858,7 +3888,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -3866,7 +3896,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -3874,7 +3904,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -3882,15 +3912,15 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="C12" s="2" t="s">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3915,17 +3945,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>115</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="B4" s="1" t="s">
-        <x:v>117</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -3933,34 +3963,34 @@
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="C6" s="2" t="s">
-        <x:v>118</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="C7" s="2" t="s">
-        <x:v>120</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
       <x:c r="C8" s="2" t="s">
-        <x:v>122</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="C9" s="2" t="s">
-        <x:v>124</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3985,17 +4015,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:6">
       <x:c r="A1" s="1" t="s">
-        <x:v>126</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6">
       <x:c r="B2" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6">
       <x:c r="B4" s="1" t="s">
-        <x:v>128</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
@@ -4006,36 +4036,36 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
       <x:c r="D7" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E7" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="D8" s="4" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E8" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
       <x:c r="D9" s="4" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E9" s="4" t="s">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6">
       <x:c r="D10" s="4" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="E10" s="6">
         <x:v>26581</x:v>
@@ -4046,36 +4076,36 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="D12" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E12" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:6">
       <x:c r="D13" s="4" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E13" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:6">
       <x:c r="D14" s="4" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E14" s="4" t="s">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:6">
       <x:c r="D15" s="4" t="s">
-        <x:v>138</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="E15" s="6">
         <x:v>26552</x:v>
@@ -4086,28 +4116,28 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="D17" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E17" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:6">
       <x:c r="D18" s="4" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E18" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:6">
       <x:c r="D19" s="4" t="s">
-        <x:v>138</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="E19" s="6">
         <x:v>26552</x:v>
@@ -4115,39 +4145,39 @@
     </x:row>
     <x:row r="20" spans="1:6">
       <x:c r="C20" s="2" t="s">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:6">
       <x:c r="D21" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E21" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:6">
       <x:c r="D22" s="4" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E22" s="4" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:6">
       <x:c r="D23" s="4" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E23" s="4" t="s">
-        <x:v>141</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:6">
       <x:c r="D24" s="4" t="s">
-        <x:v>138</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="E24" s="6">
         <x:v>27282</x:v>
@@ -4155,7 +4185,7 @@
     </x:row>
     <x:row r="26" spans="1:6">
       <x:c r="B26" s="1" t="s">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:6">
@@ -4166,26 +4196,26 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="D29" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E29" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F29" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:6">
       <x:c r="D30" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E30" s="4" t="s">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F30" s="6">
         <x:v>26581</x:v>
@@ -4193,10 +4223,10 @@
     </x:row>
     <x:row r="31" spans="1:6">
       <x:c r="D31" s="4" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E31" s="4" t="s">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F31" s="6">
         <x:v>28126</x:v>
@@ -4204,10 +4234,10 @@
     </x:row>
     <x:row r="32" spans="1:6">
       <x:c r="D32" s="4" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E32" s="4" t="s">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F32" s="6">
         <x:v>27123</x:v>
@@ -4218,26 +4248,26 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="D34" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E34" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F34" s="3" t="s">
-        <x:v>138</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:6">
       <x:c r="D35" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E35" s="4" t="s">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F35" s="6">
         <x:v>26552</x:v>
@@ -4245,10 +4275,10 @@
     </x:row>
     <x:row r="36" spans="1:6">
       <x:c r="D36" s="4" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E36" s="4" t="s">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F36" s="6">
         <x:v>28126</x:v>
@@ -4256,10 +4286,10 @@
     </x:row>
     <x:row r="37" spans="1:6">
       <x:c r="D37" s="4" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E37" s="4" t="s">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F37" s="6">
         <x:v>27123</x:v>
@@ -4267,29 +4297,29 @@
     </x:row>
     <x:row r="38" spans="1:6">
       <x:c r="C38" s="2" t="s">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D38" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:6">
       <x:c r="D39" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E39" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F39" s="3" t="s">
-        <x:v>138</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:6">
       <x:c r="D40" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E40" s="4" t="s">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F40" s="6">
         <x:v>26552</x:v>
@@ -4297,10 +4327,10 @@
     </x:row>
     <x:row r="41" spans="1:6">
       <x:c r="D41" s="4" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E41" s="4" t="s">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F41" s="6">
         <x:v>28126</x:v>
@@ -4328,17 +4358,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:35">
       <x:c r="A1" s="1" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:35">
       <x:c r="B2" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:35">
       <x:c r="B4" s="1" t="s">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:35">
@@ -4349,29 +4379,29 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:35">
       <x:c r="D7" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E7" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F7" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G7" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:35">
       <x:c r="D8" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E8" s="4" t="s">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F8" s="6">
         <x:v>26581</x:v>
@@ -4382,10 +4412,10 @@
     </x:row>
     <x:row r="9" spans="1:35">
       <x:c r="D9" s="4" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E9" s="4" t="s">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F9" s="6">
         <x:v>28126</x:v>
@@ -4396,10 +4426,10 @@
     </x:row>
     <x:row r="10" spans="1:35">
       <x:c r="D10" s="4" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E10" s="4" t="s">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F10" s="6">
         <x:v>27123</x:v>
@@ -4413,7 +4443,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:35">
@@ -4421,29 +4451,29 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:35">
       <x:c r="D13" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E13" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F13" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G13" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:35">
       <x:c r="D14" s="4" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E14" s="4" t="s">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F14" s="6">
         <x:v>27123</x:v>
@@ -4454,7 +4484,7 @@
     </x:row>
     <x:row r="16" spans="1:35">
       <x:c r="B16" s="1" t="s">
-        <x:v>156</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:35">
@@ -4465,29 +4495,29 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:35">
       <x:c r="D19" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E19" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F19" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G19" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:35">
       <x:c r="D20" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E20" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F20" s="6">
         <x:v>26581</x:v>
@@ -4498,10 +4528,10 @@
     </x:row>
     <x:row r="21" spans="1:35">
       <x:c r="D21" s="4" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E21" s="4" t="s">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F21" s="6">
         <x:v>28126</x:v>
@@ -4512,10 +4542,10 @@
     </x:row>
     <x:row r="22" spans="1:35">
       <x:c r="D22" s="4" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E22" s="4" t="s">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F22" s="6">
         <x:v>27123</x:v>
@@ -4529,7 +4559,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:35">
@@ -4537,29 +4567,29 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:35">
       <x:c r="D25" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E25" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F25" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G25" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:35">
       <x:c r="D26" s="4" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E26" s="4" t="s">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F26" s="6">
         <x:v>27123</x:v>
@@ -4570,7 +4600,7 @@
     </x:row>
     <x:row r="28" spans="1:35">
       <x:c r="B28" s="1" t="s">
-        <x:v>159</x:v>
+        <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:35">
@@ -4581,36 +4611,36 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:35">
       <x:c r="D31" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E31" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:35">
       <x:c r="D32" s="4" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E32" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:35">
       <x:c r="D33" s="4" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E33" s="4" t="s">
-        <x:v>141</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:35">
       <x:c r="D34" s="4" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="E34" s="6">
         <x:v>26581</x:v>
@@ -4618,7 +4648,7 @@
     </x:row>
     <x:row r="35" spans="1:35">
       <x:c r="D35" s="4" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="E35" s="4" t="n">
         <x:v>100</x:v>
@@ -4629,29 +4659,29 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D36" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:35">
       <x:c r="D37" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E37" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F37" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G37" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:35">
       <x:c r="D38" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E38" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F38" s="6">
         <x:v>26581</x:v>
@@ -4662,7 +4692,7 @@
     </x:row>
     <x:row r="40" spans="1:35">
       <x:c r="B40" s="1" t="s">
-        <x:v>161</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:35">
@@ -4673,113 +4703,113 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D42" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:35">
       <x:c r="D43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="H43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="I43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="J43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="K43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="L43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="M43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="N43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="O43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="P43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="Q43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="R43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="S43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="T43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="U43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="V43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="W43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="X43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="Y43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="Z43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="AA43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="AB43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="AC43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="AD43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="AE43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="AF43" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="AG43" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="AH43" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="AI43" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:35">
       <x:c r="D44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F44" s="6">
         <x:v>26552</x:v>
@@ -4788,10 +4818,10 @@
         <x:v>1000</x:v>
       </x:c>
       <x:c r="H44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="I44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="J44" s="6">
         <x:v>26552</x:v>
@@ -4800,10 +4830,10 @@
         <x:v>1000</x:v>
       </x:c>
       <x:c r="L44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="M44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="N44" s="6">
         <x:v>26552</x:v>
@@ -4812,10 +4842,10 @@
         <x:v>1000</x:v>
       </x:c>
       <x:c r="P44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="Q44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="R44" s="6">
         <x:v>26552</x:v>
@@ -4824,10 +4854,10 @@
         <x:v>1000</x:v>
       </x:c>
       <x:c r="T44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="U44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="V44" s="6">
         <x:v>26552</x:v>
@@ -4836,10 +4866,10 @@
         <x:v>1000</x:v>
       </x:c>
       <x:c r="X44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="Y44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="Z44" s="6">
         <x:v>26552</x:v>
@@ -4848,10 +4878,10 @@
         <x:v>1000</x:v>
       </x:c>
       <x:c r="AB44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="AC44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="AD44" s="6">
         <x:v>26552</x:v>
@@ -4860,10 +4890,10 @@
         <x:v>1000</x:v>
       </x:c>
       <x:c r="AF44" s="4" t="s">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="AG44" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="AH44" s="6">
         <x:v>26552</x:v>
@@ -4886,7 +4916,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D12"/>
+  <x:dimension ref="A1:D17"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -4894,36 +4924,34 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="B2" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
-      <x:c r="B4" s="1" t="s">
-        <x:v>165</x:v>
-      </x:c>
+      <x:c r="B4" s="1" t="s"/>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="C5" s="0" t="s"/>
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="C6" s="2" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="C7" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -4939,7 +4967,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
@@ -4947,7 +4975,31 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="B14" s="1" t="s">
         <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="C15" s="0" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="C16" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="C17" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>172</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -4972,17 +5024,17 @@
   <x:sheetData>
     <x:row r="1" spans="1:6">
       <x:c r="A1" s="1" t="s">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6">
       <x:c r="B2" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6">
       <x:c r="B4" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
@@ -4993,7 +5045,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
@@ -5001,7 +5053,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
@@ -5009,7 +5061,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
@@ -5017,24 +5069,24 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="B11" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="C12" s="0" t="s"/>
       <x:c r="D12" s="3" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="E12" s="3" t="s">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F12" s="3" t="s">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:6">
@@ -5072,19 +5124,19 @@
     </x:row>
     <x:row r="16" spans="1:6">
       <x:c r="B16" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="C17" s="0" t="s"/>
       <x:c r="D17" s="3" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="E17" s="3" t="s">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F17" s="3" t="s">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:6">
@@ -5111,7 +5163,7 @@
     </x:row>
     <x:row r="21" spans="1:6">
       <x:c r="B21" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:6">
@@ -5122,7 +5174,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:6">
@@ -5130,7 +5182,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:6">
@@ -5138,7 +5190,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:6">
@@ -5146,24 +5198,24 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:6">
       <x:c r="B28" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="C29" s="0" t="s"/>
       <x:c r="D29" s="3" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="E29" s="3" t="s">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F29" s="3" t="s">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:6">
@@ -5201,19 +5253,19 @@
     </x:row>
     <x:row r="33" spans="1:6">
       <x:c r="B33" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="C34" s="0" t="s"/>
       <x:c r="D34" s="3" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="E34" s="3" t="s">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F34" s="3" t="s">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:6">

</xml_diff>

<commit_message>
Add output of version 1.1.0
</commit_message>
<xml_diff>
--- a/Output/Excel/features.xlsx
+++ b/Output/Excel/features.xlsx
@@ -1151,61 +1151,61 @@
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="8">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="8">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>

<commit_message>
Output for version 2.0.0
</commit_message>
<xml_diff>
--- a/Output/Excel/features.xlsx
+++ b/Output/Excel/features.xlsx
@@ -41,9 +41,9 @@
     <x:t>Clearing Screen</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to restart a new set of calculations
-As a math idiot
-I want to be able to clear the screen</x:t>
+    <x:t xml:space="preserve">	In order to restart a new set of calculations
+	As a math idiot
+	I want to be able to clear the screen</x:t>
   </x:si>
   <x:si>
     <x:t>Clear the screen</x:t>
@@ -76,10 +76,10 @@
     <x:t>Interactive DHTML View</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to increase stakeholder engagement with pickled specs
-As a SpecFlow evangelist  
-I want to adjust the level of detail in the DHTML view to suit my audience
-So that I do not overwhelm them.</x:t>
+    <x:t xml:space="preserve">	In order to increase stakeholder engagement with pickled specs
+	As a SpecFlow evangelist  
+	I want to adjust the level of detail in the DHTML view to suit my audience
+	So that I do not overwhelm them.</x:t>
   </x:si>
   <x:si>
     <x:t>Scenario with large data table</x:t>
@@ -169,29 +169,29 @@
     <x:t>Sample Markdown Feature</x:t>
   </x:si>
   <x:si>
-    <x:t>Header 1
-========
-Header 2
---------
-This is a *significant* word
-1. Ordered #1
-2. Ordered #2
-3. Ordered #3
-- Unordered #1 
-- Unordered #2
-- Unordered #3 	
-Horizontal Rule:  
-- - -
-Table example:  
-| First Header  | Second Header |
-| ------------- | ------------- |
-| Content Cell  | Content Cell  |
-| Content Cell  | Content Cell  | 
-- - -
+    <x:t xml:space="preserve">	Header 1
+	========
+	Header 2
+	--------
+	This is a *significant* word
+	1. Ordered #1
+	2. Ordered #2
+	3. Ordered #3
+	- Unordered #1 
+	- Unordered #2
+	- Unordered #3 	
+	Horizontal Rule:  
+	- - -
+	Table example:  
+	| First Header  | Second Header |
+	| ------------- | ------------- |
+	| Content Cell  | Content Cell  |
+	| Content Cell  | Content Cell  | 
+	- - -
 Including a picture: ![](./image.png)</x:t>
   </x:si>
   <x:si>
-    <x:t>This is the *coolest* background</x:t>
+    <x:t xml:space="preserve">		This is the *coolest* background</x:t>
   </x:si>
   <x:si>
     <x:t>I have initialized the Sum-variable to 0</x:t>
@@ -203,18 +203,17 @@
     <x:t>Sample Markdown Scenario Example</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">
-This is **important** text
-Code Block:  
-```
-var x = 2;
-```
-Apple
-:   Pomaceous fruit of plants of the genus Malus in 
-the family Rosaceae.
-:   An American computer company.
-Orange
-:   The fruit of an evergreen tree of the genus Citrus.</x:t>
+    <x:t xml:space="preserve">		This is **important** text
+		Code Block:  
+		```
+		var x = 2;
+		```
+		Apple
+		:   Pomaceous fruit of plants of the genus Malus in 
+			the family Rosaceae.
+		:   An American computer company.
+		Orange
+		:   The fruit of an evergreen tree of the genus Citrus.</x:t>
   </x:si>
   <x:si>
     <x:t>this</x:t>
@@ -226,9 +225,8 @@
     <x:t>Sample Markdown Scenario Outline Example</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">
-This is [an example link to pickles](https://github.com/picklesdoc/pickles/wiki "Pickles") inline link.
-[This link to pickles](https://github.com/picklesdoc/pickles/wiki) has no title attribute.</x:t>
+    <x:t xml:space="preserve">		This is [an example link to pickles](https://github.com/picklesdoc/pickles/wiki "Pickles") inline link.
+		[This link to pickles](https://github.com/picklesdoc/pickles/wiki) has no title attribute.</x:t>
   </x:si>
   <x:si>
     <x:t>this: &lt;test&gt;</x:t>
@@ -240,8 +238,7 @@
     <x:t>Examples</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">
-This __message__ is important too and is for an *Example* table.</x:t>
+    <x:t xml:space="preserve">			This __message__ is important too and is for an *Example* table.</x:t>
   </x:si>
   <x:si>
     <x:t>test</x:t>
@@ -259,9 +256,9 @@
     <x:t>Multiline Feature Example</x:t>
   </x:si>
   <x:si>
-    <x:t>In order capture this particular Gherkin feature
-As a Pickles contributer
-I want to demonstrate an example of using multiline text in a Scenario</x:t>
+    <x:t xml:space="preserve">	In order capture this particular Gherkin feature
+	As a Pickles contributer
+	I want to demonstrate an example of using multiline text in a Scenario</x:t>
   </x:si>
   <x:si>
     <x:t>Mutliline Output</x:t>
@@ -288,9 +285,9 @@
     <x:t>Nested Folder Example</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to test nested folder output
-As a silly contributer
-I want to create an example of something several folders deep</x:t>
+    <x:t xml:space="preserve">	In order to test nested folder output
+	As a silly contributer
+	I want to create an example of something several folders deep</x:t>
   </x:si>
   <x:si>
     <x:t>Nested - Add two numbers</x:t>
@@ -305,11 +302,11 @@
     <x:t>Injecting context into step specifications</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to don't have to rely on the global shared state
-and to be able to define the contexts required for each scenario.
-As a SpecFlow Evanglist
-I would like to have the system automatically inject an instance of any class as 
-defined in the constructor of a step file</x:t>
+    <x:t xml:space="preserve">	In order to don't have to rely on the global shared state
+		and to be able to define the contexts required for each scenario.
+	As a SpecFlow Evanglist
+	I would like to have the system automatically inject an instance of any class as 
+		defined in the constructor of a step file</x:t>
   </x:si>
   <x:si>
     <x:t>Feature with no context</x:t>
@@ -357,9 +354,9 @@
     <x:t>Step Argument Transformations</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to reduce the amount of code and repetitive tasks in my steps
-As a SpecFlow evanglist
-I want to define reusable transformations for my step arguments</x:t>
+    <x:t xml:space="preserve">	In order to reduce the amount of code and repetitive tasks in my steps
+	As a SpecFlow evanglist
+	I want to define reusable transformations for my step arguments</x:t>
   </x:si>
   <x:si>
     <x:t>Steps with non-string arguments</x:t>
@@ -377,9 +374,9 @@
     <x:t>Calling Steps from StepDefinitions</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to create steps of a higher abstraction
-As a SpecFlow evangelist
-I want reuse other steps in my step definitions</x:t>
+    <x:t xml:space="preserve">	In order to create steps of a higher abstraction
+	As a SpecFlow evangelist
+	I want reuse other steps in my step definitions</x:t>
   </x:si>
   <x:si>
     <x:t>Log in</x:t>
@@ -412,9 +409,9 @@
     <x:t>Attribute overloading</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show that steps can be used with multiple attributes
-As a SpecFlow Evangelist
-I want to show that similar attributes can be applied to the same step definition</x:t>
+    <x:t xml:space="preserve">	In order to show that steps can be used with multiple attributes
+	As a SpecFlow Evangelist
+	I want to show that similar attributes can be applied to the same step definition</x:t>
   </x:si>
   <x:si>
     <x:t>Checking number for evenness</x:t>
@@ -447,9 +444,9 @@
     <x:t>Summering</x:t>
   </x:si>
   <x:si>
-    <x:t>För att slippa att göra dumma fel
-Som räknare
-Vill jag kunna lägga summera</x:t>
+    <x:t xml:space="preserve">	För att slippa att göra dumma fel
+	Som räknare
+	Vill jag kunna lägga summera</x:t>
   </x:si>
   <x:si>
     <x:t>Summera 5 och 7 ska vara 12</x:t>
@@ -482,9 +479,9 @@
     <x:t>Show the compare to feature</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show the compare to features of SpecFlow Assist
-As a SpecFlow evanglist
-I want to show how the different versions of compareTo works</x:t>
+    <x:t xml:space="preserve">	In order to show the compare to features of SpecFlow Assist
+	As a SpecFlow evanglist
+	I want to show how the different versions of compareTo works</x:t>
   </x:si>
   <x:si>
     <x:t>CompareToInstance</x:t>
@@ -553,9 +550,9 @@
     <x:t>Showing table usage</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show how to use tables
-As a SpecFlow evanglist
-I want to write some simple scenarios that uses tables tables</x:t>
+    <x:t xml:space="preserve">	In order to show how to use tables
+	As a SpecFlow evanglist
+	I want to write some simple scenarios that uses tables tables</x:t>
   </x:si>
   <x:si>
     <x:t>Using tables</x:t>
@@ -597,9 +594,9 @@
     <x:t>Show the use of background</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show how to use the Background keyword of Gherkin
-As a SpecFlow evanglist
-I want to show that background steps are called before any scenario step</x:t>
+    <x:t xml:space="preserve">	In order to show how to use the Background keyword of Gherkin
+	As a SpecFlow evanglist
+	I want to show that background steps are called before any scenario step</x:t>
   </x:si>
   <x:si>
     <x:t>Add 1 to the sum</x:t>
@@ -620,9 +617,9 @@
     <x:t>Scenario outline</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to not have to type the same scenario over and over
-As a SpecFlow evangelist
-I want to show how to use ScenarioOutline</x:t>
+    <x:t xml:space="preserve">	In order to not have to type the same scenario over and over
+	As a SpecFlow evangelist
+	I want to show how to use ScenarioOutline</x:t>
   </x:si>
   <x:si>
     <x:t>Add two positive numbers with many examples</x:t>
@@ -655,9 +652,9 @@
     <x:t>FeatureContext features</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show how to use FeatureContext
-As a SpecFlow evangelist
-I want to write some simple scenarios with data in FeatureContext</x:t>
+    <x:t xml:space="preserve">	In order to show how to use FeatureContext
+	As a SpecFlow evangelist
+	I want to write some simple scenarios with data in FeatureContext</x:t>
   </x:si>
   <x:si>
     <x:t>Store and retrive Person Marcus from FeatureContext Current</x:t>
@@ -708,9 +705,9 @@
     <x:t>Scenario Context features</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show how to use ScenarioContext
-As a SpecFlow evangelist
-I want to write some simple scenarios with data in ScenarioContext</x:t>
+    <x:t xml:space="preserve">	In order to show how to use ScenarioContext
+	As a SpecFlow evangelist
+	I want to write some simple scenarios with data in ScenarioContext</x:t>
   </x:si>
   <x:si>
     <x:t>Store and retrive Person Marcus from ScenarioContext</x:t>
@@ -764,9 +761,9 @@
     <x:t>Tag demonstrator</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show the capabilities of tags in SpecFlow
-As a SpecFlow evanglist
-I want to write scenarios that has tags and show their usage in code</x:t>
+    <x:t xml:space="preserve">	In order to show the capabilities of tags in SpecFlow
+	As a SpecFlow evanglist
+	I want to write scenarios that has tags and show their usage in code</x:t>
   </x:si>
   <x:si>
     <x:t>Ignored scenario</x:t>
@@ -823,9 +820,9 @@
     <x:t>Addition</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to explain the order in which hooks are run
-As a SpecFlow evanglist
-I wan to  be able to hook into pre and post conditions in SpecFlow</x:t>
+    <x:t xml:space="preserve">	In order to explain the order in which hooks are run
+	As a SpecFlow evanglist
+	I wan to  be able to hook into pre and post conditions in SpecFlow</x:t>
   </x:si>
   <x:si>
     <x:t>Hooking into pre conditions for Test Runs in SpecFlow</x:t>
@@ -864,9 +861,9 @@
     <x:t>The test runner is not (very) important</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to show that the test runner is just for the autogenerated stuff in SpecFlow  
-As a SpecFlow evanglist  
-I want to be able to call my steps in the same manner inspite of the testrunner configured</x:t>
+    <x:t xml:space="preserve">	In order to show that the test runner is just for the autogenerated stuff in SpecFlow  
+	As a SpecFlow evanglist  
+	I want to be able to call my steps in the same manner inspite of the testrunner configured  </x:t>
   </x:si>
   <x:si>
     <x:t>A couple of simple steps</x:t>
@@ -884,10 +881,10 @@
     <x:t>Showing basic gherkin syntax</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to see that gherkin is a very simple langauge  
-As a SpecFlow evangelist  
-I want to show that basic syntax  
-![Test Image](test.jpg)</x:t>
+    <x:t xml:space="preserve">	In order to see that gherkin is a very simple langauge  
+	As a SpecFlow evangelist  
+	I want to show that basic syntax  
+	![Test Image](test.jpg)</x:t>
   </x:si>
   <x:si>
     <x:t>Simple GWT</x:t>
@@ -917,9 +914,9 @@
     <x:t>Trigonometry</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to avoid perform more advanced calculations
-As a math idiot
-I want to be able to use trigonometric functions</x:t>
+    <x:t xml:space="preserve">	In order to avoid perform more advanced calculations
+	As a math idiot
+	I want to be able to use trigonometric functions</x:t>
   </x:si>
   <x:si>
     <x:t>Sine</x:t>
@@ -955,9 +952,9 @@
     <x:t>Arithmetic</x:t>
   </x:si>
   <x:si>
-    <x:t>In order to avoid silly mistakes
-As a math idiot
-I want to be able to perform arithmetic on the calculator</x:t>
+    <x:t xml:space="preserve">	In order to avoid silly mistakes
+	As a math idiot
+	I want to be able to perform arithmetic on the calculator</x:t>
   </x:si>
   <x:si>
     <x:t>Add two numbers</x:t>
@@ -3334,7 +3331,7 @@
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
-      <x:c r="C20" s="5" t="s">
+      <x:c r="C20" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
       <x:c r="D20" s="3" t="s">

</xml_diff>